<commit_message>
refactor: on save, write entire xlsx file fresh
</commit_message>
<xml_diff>
--- a/tamarin_todo.xlsx
+++ b/tamarin_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Id</t>
   </si>
@@ -31,7 +31,9 @@
     <t>Created</t>
   </si>
   <si>
-    <t>rename repository to Tamarin</t>
+    <t xml:space="preserve">major refactor step 1:
+all edits made to Project must be made to generic Project format
+on save, write the entire excel worksheets at once</t>
   </si>
   <si>
     <t>Todo</t>
@@ -40,80 +42,128 @@
     <t>Feature</t>
   </si>
   <si>
+    <t>9/13/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 2:
+load excel format into generic Project format
+don't keep the excel objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 3:
+save generic Project format to xml
+on save, if filename has xlsx extension, auto save it to filename.xml instead</t>
+  </si>
+  <si>
+    <t>update to only open/create/save new xml format</t>
+  </si>
+  <si>
     <t>9/12/2018</t>
+  </si>
+  <si>
+    <t>broke the icon again</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>update license</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cleanup documentation
+make it consistent with library projects</t>
+  </si>
+  <si>
+    <t>convert dev_notes.txt to this todo list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github use case:
+user1 adds a task, given id 5
+user2 at the same time adds a task, given id 5
+both users check in
+github merges the files
+now there are two tasks with id 5
+What validation and auto-update should Tamarin do when it next opens the file?
+this will certainly need to be documented behavior</t>
+  </si>
+  <si>
+    <t>go through Lia's test results</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>4/11/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create a custom layout manager that works better and faster
+- at the same time, refactor all forms from Design to Code</t>
+  </si>
+  <si>
+    <t>don't leave comboboxes highlighted in blue after the list is updated</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
+maybe in version 3</t>
+  </si>
+  <si>
+    <t>visual indication that a list has been edited but not saved</t>
+  </si>
+  <si>
+    <t>better icon</t>
+  </si>
+  <si>
+    <t>when adding new task to Inactive list directly, auto-select the first inactive status possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't let user save with any file format suffix other than xlsx
+- was able to save with filename x.txt</t>
+  </si>
+  <si>
+    <t>8/9/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">probably need to roll my own layout manager
+it takes WAY too long to switch lists, open lists, close lists</t>
+  </si>
+  <si>
+    <t>if only an empty "new" file is open, and user opens an actual file, then auto-close the empty file</t>
+  </si>
+  <si>
+    <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
+  </si>
+  <si>
+    <t>12/14/2017</t>
+  </si>
+  <si>
+    <t>you can move a row to a row higher than you should be able to</t>
+  </si>
+  <si>
+    <t>adding a task with Add Button does not set task height properly</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
   <si>
     <t xml:space="preserve">FOUND MAJOR FLAW IN DESIGN:
 xlsx files can't merge in Git, at least not in any meaningful way
 can I save to pure xml instead?
 that should merge ok
-I can at least read it in Notepad</t>
-  </si>
-  <si>
-    <t>broke the icon again</t>
-  </si>
-  <si>
-    <t>convert dev_notes.txt to this todo list</t>
-  </si>
-  <si>
-    <t>go through Lia's test results</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>4/11/2018</t>
-  </si>
-  <si>
-    <t>don't leave comboboxes highlighted in blue after the list is updated</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
-maybe in version 3</t>
-  </si>
-  <si>
-    <t>visual indication that a list has been edited but not saved</t>
-  </si>
-  <si>
-    <t>better icon</t>
-  </si>
-  <si>
-    <t>when adding new task to Inactive list directly, auto-select the first inactive status possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">don't let user save with any file format suffix other than xlsx
-- was able to save with filename x.txt</t>
-  </si>
-  <si>
-    <t>8/9/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">probably need to roll my own layout manager
-it takes WAY too long to switch lists, open lists, close lists</t>
-  </si>
-  <si>
-    <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
-  </si>
-  <si>
-    <t>12/14/2017</t>
-  </si>
-  <si>
-    <t>you can move a row to a row higher than you should be able to</t>
-  </si>
-  <si>
-    <t>adding a task with Add Button does not set task height properly</t>
-  </si>
-  <si>
-    <t>Done</t>
+I can at least read it in Notepad
+Yes, can save to MS Excel 2003 XML format
+- verified OpenOffice can open that</t>
+  </si>
+  <si>
+    <t>rename repository to Tamarin</t>
   </si>
   <si>
     <t xml:space="preserve">get the msi installed program to run again - it won't run after installation
@@ -276,6 +326,22 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 2:
+load excel format into generic Project format
+don't keep the excel objects
+all edits must be made to generic Project object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 2:
+load excel format into generic Project format
+don't keep the excel objects
+all edits must be made to generic Project objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 1:
+on save, write the entire excel worksheets at once</t>
   </si>
 </sst>
 </file>
@@ -328,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -354,10 +420,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -371,10 +437,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -388,10 +454,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -400,80 +466,80 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>19</v>
@@ -482,15 +548,15 @@
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>20</v>
@@ -499,86 +565,103 @@
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>34</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -587,41 +670,126 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
+        <v>41</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
+        <v>42</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>43</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>52</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>13</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>30</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>31</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +799,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -654,567 +822,627 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>50</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>21</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>1</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
         <v>3</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>73</v>
+      <c r="B32" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1463,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1243,7 +1471,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2">
@@ -1251,43 +1479,46 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: load data from xlsx to generic format, make all edits to generic format
</commit_message>
<xml_diff>
--- a/tamarin_todo.xlsx
+++ b/tamarin_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Id</t>
   </si>
@@ -342,6 +342,15 @@
   <si>
     <t xml:space="preserve">major refactor step 1:
 on save, write the entire excel worksheets at once</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactor:
+Task.Title is being used as full task description, so update the property name and the excel column name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactor:
+Task.Title is being used as full task description, so update the property name and the excel column name
+- breaking change so wil lneed new version number</t>
   </si>
 </sst>
 </file>
@@ -420,10 +429,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -437,10 +446,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -449,15 +458,15 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -466,7 +475,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -799,7 +808,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -827,10 +836,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>39</v>
@@ -847,10 +856,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>39</v>
@@ -859,18 +868,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>39</v>
@@ -887,30 +896,30 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>39</v>
@@ -919,7 +928,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>22</v>
@@ -927,19 +936,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>22</v>
@@ -947,16 +956,16 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>22</v>
@@ -967,10 +976,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>39</v>
@@ -987,19 +996,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>22</v>
@@ -1007,10 +1016,10 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>39</v>
@@ -1019,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>22</v>
@@ -1027,19 +1036,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>22</v>
@@ -1047,19 +1056,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>22</v>
@@ -1067,19 +1076,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>22</v>
@@ -1087,10 +1096,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>39</v>
@@ -1107,10 +1116,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>39</v>
@@ -1122,41 +1131,41 @@
         <v>50</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>61</v>
@@ -1167,10 +1176,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>39</v>
@@ -1179,7 +1188,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>62</v>
@@ -1187,30 +1196,30 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>39</v>
@@ -1219,7 +1228,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>68</v>
@@ -1227,19 +1236,19 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>68</v>
@@ -1247,19 +1256,19 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>68</v>
@@ -1267,10 +1276,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>39</v>
@@ -1279,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>68</v>
@@ -1287,10 +1296,10 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>39</v>
@@ -1299,7 +1308,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>68</v>
@@ -1307,19 +1316,19 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>68</v>
@@ -1327,16 +1336,16 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>45</v>
@@ -1347,10 +1356,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>39</v>
@@ -1367,10 +1376,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>39</v>
@@ -1387,10 +1396,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>39</v>
@@ -1399,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>68</v>
@@ -1407,41 +1416,61 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
+        <v>1</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
         <v>3</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B33" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="C33" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1485,7 +1514,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
always save to xml format
</commit_message>
<xml_diff>
--- a/tamarin_todo.xlsx
+++ b/tamarin_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -31,9 +31,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t xml:space="preserve">major refactor step 1:
-all edits made to Project must be made to generic Project format
-on save, write the entire excel worksheets at once</t>
+    <t>update to only open/create/save new xml format</t>
   </si>
   <si>
     <t>Todo</t>
@@ -42,23 +40,15 @@
     <t>Feature</t>
   </si>
   <si>
+    <t>9/12/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refactor:
+Task.Title is being used as full task description, so update the property name and the excel column name
+- breaking change so wil lneed new version number</t>
+  </si>
+  <si>
     <t>9/13/2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">major refactor step 2:
-load excel format into generic Project format
-don't keep the excel objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">major refactor step 3:
-save generic Project format to xml
-on save, if filename has xlsx extension, auto save it to filename.xml instead</t>
-  </si>
-  <si>
-    <t>update to only open/create/save new xml format</t>
-  </si>
-  <si>
-    <t>9/12/2018</t>
   </si>
   <si>
     <t>broke the icon again</t>
@@ -154,6 +144,21 @@
     <t>Done</t>
   </si>
   <si>
+    <t xml:space="preserve">major refactor step 3:
+save generic Project format to xml
+on save, if filename has xlsx extension, auto save it to filename.xml instead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 2:
+load excel format into generic Project format
+don't keep the excel objects
+all edits must be made to generic Project objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">major refactor step 1:
+on save, write the entire excel worksheets at once</t>
+  </si>
+  <si>
     <t xml:space="preserve">FOUND MAJOR FLAW IN DESIGN:
 xlsx files can't merge in Git, at least not in any meaningful way
 can I save to pure xml instead?
@@ -326,31 +331,6 @@
   </si>
   <si>
     <t>Inactive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">major refactor step 2:
-load excel format into generic Project format
-don't keep the excel objects
-all edits must be made to generic Project object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">major refactor step 2:
-load excel format into generic Project format
-don't keep the excel objects
-all edits must be made to generic Project objects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">major refactor step 1:
-on save, write the entire excel worksheets at once</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refactor:
-Task.Title is being used as full task description, so update the property name and the excel column name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refactor:
-Task.Title is being used as full task description, so update the property name and the excel column name
-- breaking change so wil lneed new version number</t>
   </si>
 </sst>
 </file>
@@ -403,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,10 +409,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -446,10 +426,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -458,21 +438,21 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>8</v>
@@ -480,7 +460,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -492,12 +472,12 @@
         <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>15</v>
@@ -506,117 +486,117 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>25</v>
@@ -625,35 +605,35 @@
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -662,46 +642,46 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>31</v>
@@ -710,49 +690,49 @@
         <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>13</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0">
-        <v>52</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="C21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>35</v>
@@ -761,44 +741,27 @@
         <v>6</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0">
-        <v>31</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +771,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -831,647 +794,667 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="F12" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="F21" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F24" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F27" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>78</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>80</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>81</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
+        <v>1</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
         <v>3</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="B34" s="0" t="s">
         <v>84</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1492,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1500,7 +1483,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -1508,7 +1491,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
@@ -1519,35 +1502,35 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save all files as XML format
</commit_message>
<xml_diff>
--- a/tamarin_todo.xlsx
+++ b/tamarin_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Id</t>
   </si>
@@ -31,7 +31,8 @@
     <t>Created</t>
   </si>
   <si>
-    <t>update to only open/create/save new xml format</t>
+    <t xml:space="preserve">load xml format
+in open dialog, allow xlsx and xml formats</t>
   </si>
   <si>
     <t>Todo</t>
@@ -40,7 +41,7 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>9/12/2018</t>
+    <t>9/13/2018</t>
   </si>
   <si>
     <t xml:space="preserve">refactor:
@@ -48,13 +49,13 @@
 - breaking change so wil lneed new version number</t>
   </si>
   <si>
-    <t>9/13/2018</t>
-  </si>
-  <si>
     <t>broke the icon again</t>
   </si>
   <si>
     <t>Bug</t>
+  </si>
+  <si>
+    <t>9/12/2018</t>
   </si>
   <si>
     <t>update license</t>
@@ -144,6 +145,9 @@
     <t>Done</t>
   </si>
   <si>
+    <t>update to only open/create/save new xml format</t>
+  </si>
+  <si>
     <t xml:space="preserve">major refactor step 3:
 save generic Project format to xml
 on save, if filename has xlsx extension, auto save it to filename.xml instead</t>
@@ -331,6 +335,9 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t>9/14/2018</t>
   </si>
 </sst>
 </file>
@@ -383,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,10 +416,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -426,44 +433,44 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -472,15 +479,15 @@
         <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
@@ -489,21 +496,21 @@
         <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>8</v>
@@ -511,27 +518,27 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -540,15 +547,15 @@
         <v>19</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -557,55 +564,55 @@
         <v>19</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>20</v>
@@ -613,10 +620,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -630,16 +637,16 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>20</v>
@@ -647,33 +654,33 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>30</v>
@@ -681,86 +688,69 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0">
-        <v>52</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>8</v>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>13</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="0">
-        <v>31</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="0" t="s">
         <v>20</v>
       </c>
     </row>
@@ -771,7 +761,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -799,10 +789,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>37</v>
@@ -811,18 +801,18 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>37</v>
@@ -831,18 +821,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>37</v>
@@ -851,18 +841,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>37</v>
@@ -879,10 +869,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>37</v>
@@ -899,59 +889,59 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>20</v>
@@ -959,19 +949,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>20</v>
@@ -979,16 +969,16 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>20</v>
@@ -999,19 +989,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>20</v>
@@ -1019,19 +1009,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>20</v>
@@ -1039,19 +1029,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>20</v>
@@ -1059,10 +1049,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>37</v>
@@ -1071,7 +1061,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>20</v>
@@ -1079,19 +1069,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>20</v>
@@ -1099,19 +1089,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>20</v>
@@ -1119,150 +1109,150 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>37</v>
@@ -1271,38 +1261,38 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>37</v>
@@ -1311,38 +1301,38 @@
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>37</v>
@@ -1351,38 +1341,38 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>37</v>
@@ -1391,18 +1381,18 @@
         <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>37</v>
@@ -1411,50 +1401,90 @@
         <v>7</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
+        <v>21</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>1</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
         <v>3</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="B36" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>85</v>
+      <c r="F36" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1505,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1483,7 +1513,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
@@ -1491,21 +1521,21 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>19</v>
@@ -1516,18 +1546,18 @@
         <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
rename Task.Title to Task.Description; backward compatible
</commit_message>
<xml_diff>
--- a/tamarin_todo.xlsx
+++ b/tamarin_todo.xlsx
@@ -390,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,33 +416,33 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>12</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -467,10 +467,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -484,44 +484,44 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -530,15 +530,15 @@
         <v>19</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -547,32 +547,32 @@
         <v>19</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -581,21 +581,21 @@
         <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>20</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -620,16 +620,16 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>20</v>
@@ -637,10 +637,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -649,15 +649,15 @@
         <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -671,10 +671,10 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -683,49 +683,49 @@
         <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0">
-        <v>52</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>13</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>6</v>
@@ -734,23 +734,6 @@
         <v>11</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0">
-        <v>31</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="0" t="s">
         <v>20</v>
       </c>
     </row>
@@ -761,7 +744,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -789,10 +772,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>37</v>
@@ -809,10 +792,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>37</v>
@@ -821,18 +804,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>37</v>
@@ -841,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>8</v>
@@ -849,10 +832,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>37</v>
@@ -869,10 +852,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>37</v>
@@ -889,10 +872,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>37</v>
@@ -901,18 +884,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>37</v>
@@ -929,30 +912,30 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>37</v>
@@ -961,7 +944,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>20</v>
@@ -969,19 +952,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>20</v>
@@ -989,16 +972,16 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>20</v>
@@ -1009,10 +992,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>37</v>
@@ -1029,19 +1012,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>20</v>
@@ -1049,10 +1032,10 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>37</v>
@@ -1061,7 +1044,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>20</v>
@@ -1069,19 +1052,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>20</v>
@@ -1089,19 +1072,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>20</v>
@@ -1109,19 +1092,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>20</v>
@@ -1129,10 +1112,10 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>37</v>
@@ -1149,10 +1132,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>37</v>
@@ -1164,41 +1147,41 @@
         <v>52</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>63</v>
@@ -1209,10 +1192,10 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>37</v>
@@ -1221,7 +1204,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>64</v>
@@ -1229,30 +1212,30 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>37</v>
@@ -1261,7 +1244,7 @@
         <v>7</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>70</v>
@@ -1269,19 +1252,19 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>70</v>
@@ -1289,19 +1272,19 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>70</v>
@@ -1309,10 +1292,10 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>37</v>
@@ -1321,7 +1304,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>70</v>
@@ -1329,10 +1312,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>37</v>
@@ -1341,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>70</v>
@@ -1349,19 +1332,19 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>70</v>
@@ -1369,16 +1352,16 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>47</v>
@@ -1389,10 +1372,10 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>37</v>
@@ -1409,10 +1392,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>37</v>
@@ -1429,10 +1412,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>37</v>
@@ -1441,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>70</v>
@@ -1449,41 +1432,61 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
+        <v>1</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
         <v>3</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B37" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="C37" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F37" s="0" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: change namespace to Tamarin; bug fix: icon
</commit_message>
<xml_diff>
--- a/tamarin_todo.xlsx
+++ b/tamarin_todo.xlsx
@@ -390,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,16 +416,16 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>12</v>
@@ -433,10 +433,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>6</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -467,44 +467,44 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -513,15 +513,15 @@
         <v>19</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -530,32 +530,32 @@
         <v>19</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -564,21 +564,21 @@
         <v>11</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>20</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -603,16 +603,16 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>20</v>
@@ -620,10 +620,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -632,15 +632,15 @@
         <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -654,10 +654,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -666,49 +666,49 @@
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0">
-        <v>52</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>13</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>6</v>
@@ -717,23 +717,6 @@
         <v>11</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0">
-        <v>31</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="0" t="s">
         <v>20</v>
       </c>
     </row>
@@ -744,7 +727,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -772,19 +755,19 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>91</v>
@@ -792,10 +775,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>37</v>
@@ -812,10 +795,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>37</v>
@@ -824,18 +807,18 @@
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>37</v>
@@ -844,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>8</v>
@@ -852,10 +835,10 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>37</v>
@@ -872,10 +855,10 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>37</v>
@@ -892,10 +875,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>37</v>
@@ -904,18 +887,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>37</v>
@@ -932,30 +915,30 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>37</v>
@@ -964,7 +947,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>20</v>
@@ -972,19 +955,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>20</v>
@@ -992,16 +975,16 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>20</v>
@@ -1012,10 +995,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>37</v>
@@ -1032,19 +1015,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>20</v>
@@ -1052,10 +1035,10 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>37</v>
@@ -1064,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>20</v>
@@ -1072,19 +1055,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>20</v>
@@ -1092,19 +1075,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>20</v>
@@ -1112,19 +1095,19 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>20</v>
@@ -1132,10 +1115,10 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>37</v>
@@ -1152,10 +1135,10 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>37</v>
@@ -1167,41 +1150,41 @@
         <v>52</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>63</v>
@@ -1212,10 +1195,10 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>37</v>
@@ -1224,7 +1207,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>64</v>
@@ -1232,30 +1215,30 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>37</v>
@@ -1264,7 +1247,7 @@
         <v>7</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>70</v>
@@ -1272,19 +1255,19 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>70</v>
@@ -1292,19 +1275,19 @@
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>70</v>
@@ -1312,10 +1295,10 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>37</v>
@@ -1324,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>70</v>
@@ -1332,10 +1315,10 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>37</v>
@@ -1344,7 +1327,7 @@
         <v>7</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>70</v>
@@ -1352,19 +1335,19 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>70</v>
@@ -1372,16 +1355,16 @@
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>47</v>
@@ -1392,10 +1375,10 @@
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>37</v>
@@ -1412,10 +1395,10 @@
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>37</v>
@@ -1432,10 +1415,10 @@
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>37</v>
@@ -1444,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>70</v>
@@ -1452,41 +1435,61 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
+        <v>1</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
         <v>3</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B38" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="C38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>